<commit_message>
Updatován xlsx tempalte a resources
</commit_message>
<xml_diff>
--- a/Ticketník/Resources/mytime_template.xlsx
+++ b/Ticketník/Resources/mytime_template.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\OneDrive\Prg\Ticketník.current\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ff6b34319afc1a0/Prg/Ticketník.current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{74C1D721-AA83-4DDF-8D94-CE0D4F2A15ED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{0B8FAD92-8B26-40DB-AF64-FC21E7B5DAC9}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_BB3D5BE43CA62C914C9B8C2F7B7C03C3F17DD2AF" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FC19860-3E2E-4D66-AF05-6B5DF83A9141}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="229" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1260" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Exported" sheetId="1" r:id="rId1"/>
+    <sheet name="Timecard" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Project</t>
   </si>
@@ -36,6 +28,12 @@
     <t>Project name</t>
   </si>
   <si>
+    <t>Task number</t>
+  </si>
+  <si>
+    <t>Task name</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -45,79 +43,106 @@
     <t>Comment1</t>
   </si>
   <si>
+    <t>Time from1</t>
+  </si>
+  <si>
+    <t>Time to1</t>
+  </si>
+  <si>
     <t>Tuesday</t>
   </si>
   <si>
     <t>Comment2</t>
   </si>
   <si>
+    <t>Time from2</t>
+  </si>
+  <si>
+    <t>Time to2</t>
+  </si>
+  <si>
     <t>Wednesday</t>
   </si>
   <si>
     <t>Comment3</t>
   </si>
   <si>
+    <t>Time from3</t>
+  </si>
+  <si>
+    <t>Time to3</t>
+  </si>
+  <si>
     <t>Thursday</t>
   </si>
   <si>
     <t>Comment4</t>
   </si>
   <si>
+    <t>Time from4</t>
+  </si>
+  <si>
+    <t>Time to4</t>
+  </si>
+  <si>
     <t>Friday</t>
   </si>
   <si>
     <t>Comment5</t>
   </si>
   <si>
+    <t>Time from5</t>
+  </si>
+  <si>
+    <t>Time to5</t>
+  </si>
+  <si>
     <t>Saturday</t>
   </si>
   <si>
     <t>Comment6</t>
   </si>
   <si>
+    <t>Time from6</t>
+  </si>
+  <si>
+    <t>Time to6</t>
+  </si>
+  <si>
     <t>Sunday</t>
   </si>
   <si>
     <t>Comment7</t>
   </si>
   <si>
-    <t>Task number</t>
-  </si>
-  <si>
-    <t>Task name</t>
+    <t>Time from7</t>
+  </si>
+  <si>
+    <t>Time to7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="13"/>
-      <color indexed="9"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="1"/>
     </font>
     <font>
-      <i/>
-      <sz val="13"/>
-      <color indexed="9"/>
+      <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -129,12 +154,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="8"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -142,55 +166,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="0" applyBorder="0">
-      <protection locked="0"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <protection locked="0"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -499,244 +489,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="30.125" customWidth="1"/>
-    <col min="3" max="4" width="23.375" customWidth="1"/>
-    <col min="5" max="5" width="15.875" customWidth="1"/>
-    <col min="6" max="6" width="9.375" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="12.375" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="10.125" customWidth="1"/>
-    <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="14" width="7.5" customWidth="1"/>
-    <col min="15" max="15" width="11.5" customWidth="1"/>
-    <col min="16" max="16" width="10.125" customWidth="1"/>
-    <col min="17" max="17" width="11.5" customWidth="1"/>
-    <col min="18" max="18" width="8.5" customWidth="1"/>
-    <col min="19" max="19" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="33" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-    </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-    </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-    </row>
-    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-    </row>
-    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-    </row>
-    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-    </row>
-    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8"/>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MyTime import formát + oprava updateru.
</commit_message>
<xml_diff>
--- a/Ticketník/Resources/mytime_template.xlsx
+++ b/Ticketník/Resources/mytime_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ff6b34319afc1a0/Prg/Ticketník.current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DeveloperArea\source\repos\Caesar008\Ticketnik\Ticketník\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_BB3D5BE43CA62C914C9B8C2F7B7C03C3F17DD2AF" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FC19860-3E2E-4D66-AF05-6B5DF83A9141}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BFCFE8-D292-4943-A95C-C37F8BC2BBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1260" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timecard" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <si>
-    <t>Project</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Project name</t>
   </si>
@@ -37,88 +34,22 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Comment1</t>
-  </si>
-  <si>
-    <t>Time from1</t>
-  </si>
-  <si>
-    <t>Time to1</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Comment2</t>
-  </si>
-  <si>
-    <t>Time from2</t>
-  </si>
-  <si>
-    <t>Time to2</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Comment3</t>
-  </si>
-  <si>
-    <t>Time from3</t>
-  </si>
-  <si>
-    <t>Time to3</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Comment4</t>
-  </si>
-  <si>
-    <t>Time from4</t>
-  </si>
-  <si>
-    <t>Time to4</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Comment5</t>
-  </si>
-  <si>
-    <t>Time from5</t>
-  </si>
-  <si>
-    <t>Time to5</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Comment6</t>
-  </si>
-  <si>
-    <t>Time from6</t>
-  </si>
-  <si>
-    <t>Time to6</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Comment7</t>
-  </si>
-  <si>
-    <t>Time from7</t>
-  </si>
-  <si>
-    <t>Time to7</t>
+    <t>Project number</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Time from</t>
+  </si>
+  <si>
+    <t>Time to</t>
   </si>
 </sst>
 </file>
@@ -173,7 +104,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -489,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -513,21 +444,21 @@
     <col min="20" max="33" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -543,75 +474,6 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>